<commit_message>
Update Holt-Winters to Holt
</commit_message>
<xml_diff>
--- a/data/reports/mean_price_psf_test_results_with_rank.xlsx
+++ b/data/reports/mean_price_psf_test_results_with_rank.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\GitHub\time-series-house-price-forecasting\data\reports\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C46A22-13AE-4BF4-B00D-D6CE9ACD3D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="134">
   <si>
     <t>model</t>
   </si>
@@ -139,29 +133,296 @@
     <t>SARIMAX (1, 1, 2)</t>
   </si>
   <si>
-    <t>Holt-Winters (p=11)</t>
-  </si>
-  <si>
-    <t>Holt-Winters (p=9)</t>
-  </si>
-  <si>
-    <t>Holt-Winters (p=6)</t>
-  </si>
-  <si>
-    <t>Holt-Winters (p=2)</t>
-  </si>
-  <si>
-    <t>Holt-Winters (p=10)</t>
+    <t>Holt (p=11)</t>
+  </si>
+  <si>
+    <t>Holt (p=9)</t>
+  </si>
+  <si>
+    <t>Holt (p=6)</t>
+  </si>
+  <si>
+    <t>Holt (p=2)</t>
+  </si>
+  <si>
+    <t>Holt (p=10)</t>
+  </si>
+  <si>
+    <t>674.2978055725536 (5.5)</t>
+  </si>
+  <si>
+    <t>673.6106963611131 (3.5)</t>
+  </si>
+  <si>
+    <t>664.0983390320221 (1.5)</t>
+  </si>
+  <si>
+    <t>775.3491169966069 (9.5)</t>
+  </si>
+  <si>
+    <t>777.0053157799958 (11.5)</t>
+  </si>
+  <si>
+    <t>717.3468035660213 (8.0)</t>
+  </si>
+  <si>
+    <t>810.6473067052551 (13.0)</t>
+  </si>
+  <si>
+    <t>929.9109168094712 (15.0)</t>
+  </si>
+  <si>
+    <t>818.3501750189789 (14.0)</t>
+  </si>
+  <si>
+    <t>691.131567278571 (7.0)</t>
+  </si>
+  <si>
+    <t>25.96724485910189 (5.5)</t>
+  </si>
+  <si>
+    <t>25.95401118056924 (3.5)</t>
+  </si>
+  <si>
+    <t>25.77010553009091 (1.5)</t>
+  </si>
+  <si>
+    <t>27.84509143451691 (9.5)</t>
+  </si>
+  <si>
+    <t>27.874815080642165 (11.5)</t>
+  </si>
+  <si>
+    <t>26.783330703368865 (8.0)</t>
+  </si>
+  <si>
+    <t>28.47186869008171 (13.0)</t>
+  </si>
+  <si>
+    <t>30.494440752528504 (15.0)</t>
+  </si>
+  <si>
+    <t>28.60682042833455 (14.0)</t>
+  </si>
+  <si>
+    <t>26.289381264658378 (7.0)</t>
+  </si>
+  <si>
+    <t>18.601215220846036 (5.5)</t>
+  </si>
+  <si>
+    <t>17.714811925556326 (1.5)</t>
+  </si>
+  <si>
+    <t>18.073931080708963 (3.5)</t>
+  </si>
+  <si>
+    <t>23.31571210978221 (11.5)</t>
+  </si>
+  <si>
+    <t>23.31194919011911 (9.5)</t>
+  </si>
+  <si>
+    <t>21.85345357083955 (7.0)</t>
+  </si>
+  <si>
+    <t>23.50549995279969 (13.0)</t>
+  </si>
+  <si>
+    <t>25.834170252600696 (15.0)</t>
+  </si>
+  <si>
+    <t>23.990441641161837 (14.0)</t>
+  </si>
+  <si>
+    <t>21.954650461802576 (8.0)</t>
+  </si>
+  <si>
+    <t>0.03586044842887329 (5.5)</t>
+  </si>
+  <si>
+    <t>0.034263380323902456 (1.5)</t>
+  </si>
+  <si>
+    <t>0.03492192266618972 (3.5)</t>
+  </si>
+  <si>
+    <t>0.04327788910482188 (11.5)</t>
+  </si>
+  <si>
+    <t>0.043266149042399185 (9.5)</t>
+  </si>
+  <si>
+    <t>0.04067794409124053 (7.0)</t>
+  </si>
+  <si>
+    <t>0.04367096637612008 (13.0)</t>
+  </si>
+  <si>
+    <t>0.04793940537141732 (15.0)</t>
+  </si>
+  <si>
+    <t>0.04453351824776052 (14.0)</t>
+  </si>
+  <si>
+    <t>0.040889470885861076 (8.0)</t>
+  </si>
+  <si>
+    <t>-0.38001793565055664 (5.5)</t>
+  </si>
+  <si>
+    <t>-0.37861169789076854 (3.5)</t>
+  </si>
+  <si>
+    <t>-0.35914370672132345 (1.5)</t>
+  </si>
+  <si>
+    <t>-0.5868295566194146 (9.5)</t>
+  </si>
+  <si>
+    <t>-0.5902191331643638 (11.5)</t>
+  </si>
+  <si>
+    <t>-0.46812201792964125 (8.0)</t>
+  </si>
+  <si>
+    <t>-0.6590708341252318 (13.0)</t>
+  </si>
+  <si>
+    <t>-0.903155746836021 (15.0)</t>
+  </si>
+  <si>
+    <t>-0.6748355249503297 (14.0)</t>
+  </si>
+  <si>
+    <t>-0.4144699135255936 (7.0)</t>
+  </si>
+  <si>
+    <t>81.24883171017615 (14.5)</t>
+  </si>
+  <si>
+    <t>80.28944324637376 (12.5)</t>
+  </si>
+  <si>
+    <t>79.51788448493772 (10.5)</t>
+  </si>
+  <si>
+    <t>56.51511608996168 (1.5)</t>
+  </si>
+  <si>
+    <t>56.56751991647627 (3.5)</t>
+  </si>
+  <si>
+    <t>59.76154383368828 (6.0)</t>
+  </si>
+  <si>
+    <t>60.12513732458484 (7.0)</t>
+  </si>
+  <si>
+    <t>58.7636758241826 (5.0)</t>
+  </si>
+  <si>
+    <t>60.170630607549185 (8.0)</t>
+  </si>
+  <si>
+    <t>60.91456235127316 (9.0)</t>
+  </si>
+  <si>
+    <t>0.04927236076539473 (3.5)</t>
+  </si>
+  <si>
+    <t>0.049272383100670274 (5.5)</t>
+  </si>
+  <si>
+    <t>0.04894163727341141 (1.5)</t>
+  </si>
+  <si>
+    <t>0.05252741607289062 (9.5)</t>
+  </si>
+  <si>
+    <t>0.052584195373218325 (11.5)</t>
+  </si>
+  <si>
+    <t>0.05055865498764959 (8.0)</t>
+  </si>
+  <si>
+    <t>0.05379096409979055 (13.0)</t>
+  </si>
+  <si>
+    <t>0.057750116588687284 (15.0)</t>
+  </si>
+  <si>
+    <t>0.0540277211232806 (14.0)</t>
+  </si>
+  <si>
+    <t>0.04962809820440373 (7.0)</t>
+  </si>
+  <si>
+    <t>1.2646976420181772 (5.5)</t>
+  </si>
+  <si>
+    <t>1.2627420746889129 (3.5)</t>
+  </si>
+  <si>
+    <t>1.2459655913715855 (1.5)</t>
+  </si>
+  <si>
+    <t>1.4794904441509327 (9.5)</t>
+  </si>
+  <si>
+    <t>1.4827163606225857 (11.5)</t>
+  </si>
+  <si>
+    <t>1.3689293155895106 (8.0)</t>
+  </si>
+  <si>
+    <t>1.5494363153831614 (13.0)</t>
+  </si>
+  <si>
+    <t>1.7838764332466326 (15.0)</t>
+  </si>
+  <si>
+    <t>1.5639871406672947 (14.0)</t>
+  </si>
+  <si>
+    <t>1.3181558368068218 (7.0)</t>
+  </si>
+  <si>
+    <t>0.0023742058413505815 (5.5)</t>
+  </si>
+  <si>
+    <t>0.0023693286104518483 (3.5)</t>
+  </si>
+  <si>
+    <t>0.002339794495793912 (1.5)</t>
+  </si>
+  <si>
+    <t>0.0028246869038194215 (9.5)</t>
+  </si>
+  <si>
+    <t>0.002830970287050209 (11.5)</t>
+  </si>
+  <si>
+    <t>0.002613959151235701 (8.0)</t>
+  </si>
+  <si>
+    <t>0.0029632361884829833 (13.0)</t>
+  </si>
+  <si>
+    <t>0.0034241258201082037 (15.0)</t>
+  </si>
+  <si>
+    <t>0.0029907134343519102 (14.0)</t>
+  </si>
+  <si>
+    <t>0.0025156385408683 (7.0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,64 +474,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +529,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -342,7 +563,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -377,10 +597,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,24 +772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="20" max="20" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,66 +838,66 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2">
-        <v>674.29780557255356</v>
+        <v>674.2978055725536</v>
       </c>
       <c r="C2">
-        <v>25.967244859101889</v>
+        <v>25.96724485910189</v>
       </c>
       <c r="D2">
         <v>18.60121522084604</v>
       </c>
       <c r="E2">
-        <v>3.5860448428873287E-2</v>
+        <v>0.03586044842887329</v>
       </c>
       <c r="F2">
-        <v>-0.38001793565055658</v>
+        <v>-0.3800179356505566</v>
       </c>
       <c r="G2">
-        <v>81.248831710176148</v>
+        <v>81.24883171017615</v>
       </c>
       <c r="H2">
-        <v>4.9272360765394728E-2</v>
+        <v>0.04927236076539473</v>
       </c>
       <c r="I2">
         <v>1.264697642018177</v>
       </c>
       <c r="J2">
-        <v>2.374205841350582E-3</v>
+        <v>0.002374205841350582</v>
       </c>
       <c r="K2">
         <v>5.5</v>
@@ -717,76 +926,67 @@
       <c r="S2">
         <v>5.5</v>
       </c>
-      <c r="T2" t="str">
-        <f>_xlfn.CONCAT(ROUND(B2,6)," (",K2,")")</f>
-        <v>674.297806 (5.5)</v>
-      </c>
-      <c r="U2" t="str">
-        <f t="shared" ref="U2:AB2" si="0">_xlfn.CONCAT(ROUND(C2,6)," (",L2,")")</f>
-        <v>25.967245 (5.5)</v>
-      </c>
-      <c r="V2" t="str">
-        <f t="shared" si="0"/>
-        <v>18.601215 (5.5)</v>
-      </c>
-      <c r="W2" t="str">
-        <f t="shared" si="0"/>
-        <v>0.03586 (5.5)</v>
-      </c>
-      <c r="X2" t="str">
-        <f t="shared" si="0"/>
-        <v>-0.380018 (5.5)</v>
-      </c>
-      <c r="Y2" t="str">
-        <f t="shared" si="0"/>
-        <v>81.248832 (14.5)</v>
-      </c>
-      <c r="Z2" t="str">
-        <f t="shared" si="0"/>
-        <v>0.049272 (3.5)</v>
-      </c>
-      <c r="AA2" t="str">
-        <f t="shared" si="0"/>
-        <v>1.264698 (5.5)</v>
-      </c>
-      <c r="AB2" t="str">
-        <f t="shared" si="0"/>
-        <v>0.002374 (5.5)</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>6.2777777777777777</v>
+      <c r="T2">
+        <v>6.277777777777778</v>
+      </c>
+      <c r="U2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W2" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3">
-        <v>673.61069636111313</v>
+        <v>673.6106963611131</v>
       </c>
       <c r="C3">
-        <v>25.954011180569239</v>
+        <v>25.95401118056924</v>
       </c>
       <c r="D3">
-        <v>17.714811925556329</v>
+        <v>17.71481192555633</v>
       </c>
       <c r="E3">
-        <v>3.4263380323902463E-2</v>
+        <v>0.03426338032390246</v>
       </c>
       <c r="F3">
-        <v>-0.37861169789076848</v>
+        <v>-0.3786116978907685</v>
       </c>
       <c r="G3">
-        <v>80.289443246373764</v>
+        <v>80.28944324637376</v>
       </c>
       <c r="H3">
-        <v>4.9272383100670267E-2</v>
+        <v>0.04927238310067027</v>
       </c>
       <c r="I3">
-        <v>1.2627420746889131</v>
+        <v>1.262742074688913</v>
       </c>
       <c r="J3">
-        <v>2.3693286104518479E-3</v>
+        <v>0.002369328610451848</v>
       </c>
       <c r="K3">
         <v>3.5</v>
@@ -815,76 +1015,67 @@
       <c r="S3">
         <v>3.5</v>
       </c>
-      <c r="T3" t="str">
-        <f t="shared" ref="T3:T16" si="1">_xlfn.CONCAT(ROUND(B3,6)," (",K3,")")</f>
-        <v>673.610696 (3.5)</v>
-      </c>
-      <c r="U3" t="str">
-        <f t="shared" ref="U3:U16" si="2">_xlfn.CONCAT(ROUND(C3,6)," (",L3,")")</f>
-        <v>25.954011 (3.5)</v>
-      </c>
-      <c r="V3" t="str">
-        <f t="shared" ref="V3:V16" si="3">_xlfn.CONCAT(ROUND(D3,6)," (",M3,")")</f>
-        <v>17.714812 (1.5)</v>
-      </c>
-      <c r="W3" t="str">
-        <f t="shared" ref="W3:W16" si="4">_xlfn.CONCAT(ROUND(E3,6)," (",N3,")")</f>
-        <v>0.034263 (1.5)</v>
-      </c>
-      <c r="X3" t="str">
-        <f t="shared" ref="X3:X16" si="5">_xlfn.CONCAT(ROUND(F3,6)," (",O3,")")</f>
-        <v>-0.378612 (3.5)</v>
-      </c>
-      <c r="Y3" t="str">
-        <f t="shared" ref="Y3:Y16" si="6">_xlfn.CONCAT(ROUND(G3,6)," (",P3,")")</f>
-        <v>80.289443 (12.5)</v>
-      </c>
-      <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z16" si="7">_xlfn.CONCAT(ROUND(H3,6)," (",Q3,")")</f>
-        <v>0.049272 (5.5)</v>
-      </c>
-      <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AA16" si="8">_xlfn.CONCAT(ROUND(I3,6)," (",R3,")")</f>
-        <v>1.262742 (3.5)</v>
-      </c>
-      <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB16" si="9">_xlfn.CONCAT(ROUND(J3,6)," (",S3,")")</f>
-        <v>0.002369 (3.5)</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>4.2777777777777777</v>
+      <c r="T3">
+        <v>4.277777777777778</v>
+      </c>
+      <c r="U3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4">
-        <v>664.09833903202207</v>
+        <v>664.0983390320221</v>
       </c>
       <c r="C4">
-        <v>25.770105530090909</v>
+        <v>25.77010553009091</v>
       </c>
       <c r="D4">
-        <v>18.073931080708959</v>
+        <v>18.07393108070896</v>
       </c>
       <c r="E4">
-        <v>3.4921922666189723E-2</v>
+        <v>0.03492192266618972</v>
       </c>
       <c r="F4">
-        <v>-0.35914370672132351</v>
+        <v>-0.3591437067213235</v>
       </c>
       <c r="G4">
-        <v>79.517884484937724</v>
+        <v>79.51788448493772</v>
       </c>
       <c r="H4">
-        <v>4.8941637273411408E-2</v>
+        <v>0.04894163727341141</v>
       </c>
       <c r="I4">
         <v>1.245965591371585</v>
       </c>
       <c r="J4">
-        <v>2.3397944957939121E-3</v>
+        <v>0.002339794495793912</v>
       </c>
       <c r="K4">
         <v>1.5</v>
@@ -913,76 +1104,67 @@
       <c r="S4">
         <v>1.5</v>
       </c>
-      <c r="T4" t="str">
-        <f t="shared" si="1"/>
-        <v>664.098339 (1.5)</v>
-      </c>
-      <c r="U4" t="str">
-        <f t="shared" si="2"/>
-        <v>25.770106 (1.5)</v>
-      </c>
-      <c r="V4" t="str">
-        <f t="shared" si="3"/>
-        <v>18.073931 (3.5)</v>
-      </c>
-      <c r="W4" t="str">
-        <f t="shared" si="4"/>
-        <v>0.034922 (3.5)</v>
-      </c>
-      <c r="X4" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.359144 (1.5)</v>
-      </c>
-      <c r="Y4" t="str">
-        <f t="shared" si="6"/>
-        <v>79.517884 (10.5)</v>
-      </c>
-      <c r="Z4" t="str">
-        <f t="shared" si="7"/>
-        <v>0.048942 (1.5)</v>
-      </c>
-      <c r="AA4" t="str">
-        <f t="shared" si="8"/>
-        <v>1.245966 (1.5)</v>
-      </c>
-      <c r="AB4" t="str">
-        <f t="shared" si="9"/>
-        <v>0.00234 (1.5)</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>2.9444444444444451</v>
+      <c r="T4">
+        <v>2.944444444444445</v>
+      </c>
+      <c r="U4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" t="s">
+        <v>66</v>
+      </c>
+      <c r="X4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>32</v>
       </c>
       <c r="B5">
-        <v>775.34911699660688</v>
+        <v>775.3491169966069</v>
       </c>
       <c r="C5">
         <v>27.84509143451691</v>
       </c>
       <c r="D5">
-        <v>23.315712109782211</v>
+        <v>23.31571210978221</v>
       </c>
       <c r="E5">
-        <v>4.327788910482188E-2</v>
+        <v>0.04327788910482188</v>
       </c>
       <c r="F5">
-        <v>-0.58682955661941461</v>
+        <v>-0.5868295566194146</v>
       </c>
       <c r="G5">
         <v>56.51511608996168</v>
       </c>
       <c r="H5">
-        <v>5.2527416072890618E-2</v>
+        <v>0.05252741607289062</v>
       </c>
       <c r="I5">
-        <v>1.4794904441509329</v>
+        <v>1.479490444150933</v>
       </c>
       <c r="J5">
-        <v>2.8246869038194219E-3</v>
+        <v>0.002824686903819422</v>
       </c>
       <c r="K5">
         <v>9.5</v>
@@ -1011,76 +1193,67 @@
       <c r="S5">
         <v>9.5</v>
       </c>
-      <c r="T5" t="str">
-        <f t="shared" si="1"/>
-        <v>775.349117 (9.5)</v>
-      </c>
-      <c r="U5" t="str">
-        <f t="shared" si="2"/>
-        <v>27.845091 (9.5)</v>
-      </c>
-      <c r="V5" t="str">
-        <f t="shared" si="3"/>
-        <v>23.315712 (11.5)</v>
-      </c>
-      <c r="W5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.043278 (11.5)</v>
-      </c>
-      <c r="X5" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.58683 (9.5)</v>
-      </c>
-      <c r="Y5" t="str">
-        <f t="shared" si="6"/>
-        <v>56.515116 (1.5)</v>
-      </c>
-      <c r="Z5" t="str">
-        <f t="shared" si="7"/>
-        <v>0.052527 (9.5)</v>
-      </c>
-      <c r="AA5" t="str">
-        <f t="shared" si="8"/>
-        <v>1.47949 (9.5)</v>
-      </c>
-      <c r="AB5" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002825 (9.5)</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>9.0555555555555554</v>
+      <c r="T5">
+        <v>9.055555555555555</v>
+      </c>
+      <c r="U5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V5" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" t="s">
+        <v>67</v>
+      </c>
+      <c r="X5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6">
-        <v>777.00531577999584</v>
+        <v>777.0053157799958</v>
       </c>
       <c r="C6">
-        <v>27.874815080642161</v>
+        <v>27.87481508064216</v>
       </c>
       <c r="D6">
-        <v>23.311949190119108</v>
+        <v>23.31194919011911</v>
       </c>
       <c r="E6">
-        <v>4.3266149042399192E-2</v>
+        <v>0.04326614904239919</v>
       </c>
       <c r="F6">
-        <v>-0.59021913316436381</v>
+        <v>-0.5902191331643638</v>
       </c>
       <c r="G6">
-        <v>56.567519916476272</v>
+        <v>56.56751991647627</v>
       </c>
       <c r="H6">
-        <v>5.2584195373218318E-2</v>
+        <v>0.05258419537321832</v>
       </c>
       <c r="I6">
-        <v>1.4827163606225859</v>
+        <v>1.482716360622586</v>
       </c>
       <c r="J6">
-        <v>2.8309702870502091E-3</v>
+        <v>0.002830970287050209</v>
       </c>
       <c r="K6">
         <v>11.5</v>
@@ -1109,76 +1282,67 @@
       <c r="S6">
         <v>11.5</v>
       </c>
-      <c r="T6" t="str">
-        <f t="shared" si="1"/>
-        <v>777.005316 (11.5)</v>
-      </c>
-      <c r="U6" t="str">
-        <f t="shared" si="2"/>
-        <v>27.874815 (11.5)</v>
-      </c>
-      <c r="V6" t="str">
-        <f t="shared" si="3"/>
-        <v>23.311949 (9.5)</v>
-      </c>
-      <c r="W6" t="str">
-        <f t="shared" si="4"/>
-        <v>0.043266 (9.5)</v>
-      </c>
-      <c r="X6" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.590219 (11.5)</v>
-      </c>
-      <c r="Y6" t="str">
-        <f t="shared" si="6"/>
-        <v>56.56752 (3.5)</v>
-      </c>
-      <c r="Z6" t="str">
-        <f t="shared" si="7"/>
-        <v>0.052584 (11.5)</v>
-      </c>
-      <c r="AA6" t="str">
-        <f t="shared" si="8"/>
-        <v>1.482716 (11.5)</v>
-      </c>
-      <c r="AB6" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002831 (11.5)</v>
-      </c>
-      <c r="AC6" s="2">
+      <c r="T6">
         <v>10.16666666666667</v>
       </c>
+      <c r="U6" t="s">
+        <v>48</v>
+      </c>
+      <c r="V6" t="s">
+        <v>58</v>
+      </c>
+      <c r="W6" t="s">
+        <v>68</v>
+      </c>
+      <c r="X6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7">
-        <v>674.29780557255356</v>
+        <v>674.2978055725536</v>
       </c>
       <c r="C7">
-        <v>25.967244859101889</v>
+        <v>25.96724485910189</v>
       </c>
       <c r="D7">
         <v>18.60121522084604</v>
       </c>
       <c r="E7">
-        <v>3.5860448428873287E-2</v>
+        <v>0.03586044842887329</v>
       </c>
       <c r="F7">
-        <v>-0.38001793565055658</v>
+        <v>-0.3800179356505566</v>
       </c>
       <c r="G7">
-        <v>81.248831710176148</v>
+        <v>81.24883171017615</v>
       </c>
       <c r="H7">
-        <v>4.9272360765394728E-2</v>
+        <v>0.04927236076539473</v>
       </c>
       <c r="I7">
         <v>1.264697642018177</v>
       </c>
       <c r="J7">
-        <v>2.374205841350582E-3</v>
+        <v>0.002374205841350582</v>
       </c>
       <c r="K7">
         <v>5.5</v>
@@ -1207,76 +1371,67 @@
       <c r="S7">
         <v>5.5</v>
       </c>
-      <c r="T7" t="str">
-        <f t="shared" si="1"/>
-        <v>674.297806 (5.5)</v>
-      </c>
-      <c r="U7" t="str">
-        <f t="shared" si="2"/>
-        <v>25.967245 (5.5)</v>
-      </c>
-      <c r="V7" t="str">
-        <f t="shared" si="3"/>
-        <v>18.601215 (5.5)</v>
-      </c>
-      <c r="W7" t="str">
-        <f t="shared" si="4"/>
-        <v>0.03586 (5.5)</v>
-      </c>
-      <c r="X7" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.380018 (5.5)</v>
-      </c>
-      <c r="Y7" t="str">
-        <f t="shared" si="6"/>
-        <v>81.248832 (14.5)</v>
-      </c>
-      <c r="Z7" t="str">
-        <f t="shared" si="7"/>
-        <v>0.049272 (3.5)</v>
-      </c>
-      <c r="AA7" t="str">
-        <f t="shared" si="8"/>
-        <v>1.264698 (5.5)</v>
-      </c>
-      <c r="AB7" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002374 (5.5)</v>
-      </c>
-      <c r="AC7" s="2">
-        <v>6.2777777777777777</v>
+      <c r="T7">
+        <v>6.277777777777778</v>
+      </c>
+      <c r="U7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" t="s">
+        <v>54</v>
+      </c>
+      <c r="W7" t="s">
+        <v>64</v>
+      </c>
+      <c r="X7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>35</v>
       </c>
       <c r="B8">
-        <v>673.61069636111313</v>
+        <v>673.6106963611131</v>
       </c>
       <c r="C8">
-        <v>25.954011180569239</v>
+        <v>25.95401118056924</v>
       </c>
       <c r="D8">
-        <v>17.714811925556329</v>
+        <v>17.71481192555633</v>
       </c>
       <c r="E8">
-        <v>3.4263380323902463E-2</v>
+        <v>0.03426338032390246</v>
       </c>
       <c r="F8">
-        <v>-0.37861169789076848</v>
+        <v>-0.3786116978907685</v>
       </c>
       <c r="G8">
-        <v>80.289443246373764</v>
+        <v>80.28944324637376</v>
       </c>
       <c r="H8">
-        <v>4.9272383100670267E-2</v>
+        <v>0.04927238310067027</v>
       </c>
       <c r="I8">
-        <v>1.2627420746889131</v>
+        <v>1.262742074688913</v>
       </c>
       <c r="J8">
-        <v>2.3693286104518479E-3</v>
+        <v>0.002369328610451848</v>
       </c>
       <c r="K8">
         <v>3.5</v>
@@ -1305,76 +1460,67 @@
       <c r="S8">
         <v>3.5</v>
       </c>
-      <c r="T8" t="str">
-        <f t="shared" si="1"/>
-        <v>673.610696 (3.5)</v>
-      </c>
-      <c r="U8" t="str">
-        <f t="shared" si="2"/>
-        <v>25.954011 (3.5)</v>
-      </c>
-      <c r="V8" t="str">
-        <f t="shared" si="3"/>
-        <v>17.714812 (1.5)</v>
-      </c>
-      <c r="W8" t="str">
-        <f t="shared" si="4"/>
-        <v>0.034263 (1.5)</v>
-      </c>
-      <c r="X8" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.378612 (3.5)</v>
-      </c>
-      <c r="Y8" t="str">
-        <f t="shared" si="6"/>
-        <v>80.289443 (12.5)</v>
-      </c>
-      <c r="Z8" t="str">
-        <f t="shared" si="7"/>
-        <v>0.049272 (5.5)</v>
-      </c>
-      <c r="AA8" t="str">
-        <f t="shared" si="8"/>
-        <v>1.262742 (3.5)</v>
-      </c>
-      <c r="AB8" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002369 (3.5)</v>
-      </c>
-      <c r="AC8" s="2">
-        <v>4.2777777777777777</v>
+      <c r="T8">
+        <v>4.277777777777778</v>
+      </c>
+      <c r="U8" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" t="s">
+        <v>55</v>
+      </c>
+      <c r="W8" t="s">
+        <v>65</v>
+      </c>
+      <c r="X8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>36</v>
       </c>
       <c r="B9">
-        <v>664.09833903202207</v>
+        <v>664.0983390320221</v>
       </c>
       <c r="C9">
-        <v>25.770105530090909</v>
+        <v>25.77010553009091</v>
       </c>
       <c r="D9">
-        <v>18.073931080708959</v>
+        <v>18.07393108070896</v>
       </c>
       <c r="E9">
-        <v>3.4921922666189723E-2</v>
+        <v>0.03492192266618972</v>
       </c>
       <c r="F9">
-        <v>-0.35914370672132351</v>
+        <v>-0.3591437067213235</v>
       </c>
       <c r="G9">
-        <v>79.517884484937724</v>
+        <v>79.51788448493772</v>
       </c>
       <c r="H9">
-        <v>4.8941637273411408E-2</v>
+        <v>0.04894163727341141</v>
       </c>
       <c r="I9">
         <v>1.245965591371585</v>
       </c>
       <c r="J9">
-        <v>2.3397944957939121E-3</v>
+        <v>0.002339794495793912</v>
       </c>
       <c r="K9">
         <v>1.5</v>
@@ -1403,76 +1549,67 @@
       <c r="S9">
         <v>1.5</v>
       </c>
-      <c r="T9" t="str">
-        <f t="shared" si="1"/>
-        <v>664.098339 (1.5)</v>
-      </c>
-      <c r="U9" t="str">
-        <f t="shared" si="2"/>
-        <v>25.770106 (1.5)</v>
-      </c>
-      <c r="V9" t="str">
-        <f t="shared" si="3"/>
-        <v>18.073931 (3.5)</v>
-      </c>
-      <c r="W9" t="str">
-        <f t="shared" si="4"/>
-        <v>0.034922 (3.5)</v>
-      </c>
-      <c r="X9" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.359144 (1.5)</v>
-      </c>
-      <c r="Y9" t="str">
-        <f t="shared" si="6"/>
-        <v>79.517884 (10.5)</v>
-      </c>
-      <c r="Z9" t="str">
-        <f t="shared" si="7"/>
-        <v>0.048942 (1.5)</v>
-      </c>
-      <c r="AA9" t="str">
-        <f t="shared" si="8"/>
-        <v>1.245966 (1.5)</v>
-      </c>
-      <c r="AB9" t="str">
-        <f t="shared" si="9"/>
-        <v>0.00234 (1.5)</v>
-      </c>
-      <c r="AC9" s="2">
-        <v>2.9444444444444451</v>
+      <c r="T9">
+        <v>2.944444444444445</v>
+      </c>
+      <c r="U9" t="s">
+        <v>46</v>
+      </c>
+      <c r="V9" t="s">
+        <v>56</v>
+      </c>
+      <c r="W9" t="s">
+        <v>66</v>
+      </c>
+      <c r="X9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>37</v>
       </c>
       <c r="B10">
-        <v>775.34911699660688</v>
+        <v>775.3491169966069</v>
       </c>
       <c r="C10">
         <v>27.84509143451691</v>
       </c>
       <c r="D10">
-        <v>23.315712109782211</v>
+        <v>23.31571210978221</v>
       </c>
       <c r="E10">
-        <v>4.327788910482188E-2</v>
+        <v>0.04327788910482188</v>
       </c>
       <c r="F10">
-        <v>-0.58682955661941461</v>
+        <v>-0.5868295566194146</v>
       </c>
       <c r="G10">
         <v>56.51511608996168</v>
       </c>
       <c r="H10">
-        <v>5.2527416072890618E-2</v>
+        <v>0.05252741607289062</v>
       </c>
       <c r="I10">
-        <v>1.4794904441509329</v>
+        <v>1.479490444150933</v>
       </c>
       <c r="J10">
-        <v>2.8246869038194219E-3</v>
+        <v>0.002824686903819422</v>
       </c>
       <c r="K10">
         <v>9.5</v>
@@ -1501,76 +1638,67 @@
       <c r="S10">
         <v>9.5</v>
       </c>
-      <c r="T10" t="str">
-        <f t="shared" si="1"/>
-        <v>775.349117 (9.5)</v>
-      </c>
-      <c r="U10" t="str">
-        <f t="shared" si="2"/>
-        <v>27.845091 (9.5)</v>
-      </c>
-      <c r="V10" t="str">
-        <f t="shared" si="3"/>
-        <v>23.315712 (11.5)</v>
-      </c>
-      <c r="W10" t="str">
-        <f t="shared" si="4"/>
-        <v>0.043278 (11.5)</v>
-      </c>
-      <c r="X10" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.58683 (9.5)</v>
-      </c>
-      <c r="Y10" t="str">
-        <f t="shared" si="6"/>
-        <v>56.515116 (1.5)</v>
-      </c>
-      <c r="Z10" t="str">
-        <f t="shared" si="7"/>
-        <v>0.052527 (9.5)</v>
-      </c>
-      <c r="AA10" t="str">
-        <f t="shared" si="8"/>
-        <v>1.47949 (9.5)</v>
-      </c>
-      <c r="AB10" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002825 (9.5)</v>
-      </c>
-      <c r="AC10" s="2">
-        <v>9.0555555555555554</v>
+      <c r="T10">
+        <v>9.055555555555555</v>
+      </c>
+      <c r="U10" t="s">
+        <v>47</v>
+      </c>
+      <c r="V10" t="s">
+        <v>57</v>
+      </c>
+      <c r="W10" t="s">
+        <v>67</v>
+      </c>
+      <c r="X10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>38</v>
       </c>
       <c r="B11">
-        <v>777.00531577999584</v>
+        <v>777.0053157799958</v>
       </c>
       <c r="C11">
-        <v>27.874815080642161</v>
+        <v>27.87481508064216</v>
       </c>
       <c r="D11">
-        <v>23.311949190119108</v>
+        <v>23.31194919011911</v>
       </c>
       <c r="E11">
-        <v>4.3266149042399192E-2</v>
+        <v>0.04326614904239919</v>
       </c>
       <c r="F11">
-        <v>-0.59021913316436381</v>
+        <v>-0.5902191331643638</v>
       </c>
       <c r="G11">
-        <v>56.567519916476272</v>
+        <v>56.56751991647627</v>
       </c>
       <c r="H11">
-        <v>5.2584195373218318E-2</v>
+        <v>0.05258419537321832</v>
       </c>
       <c r="I11">
-        <v>1.4827163606225859</v>
+        <v>1.482716360622586</v>
       </c>
       <c r="J11">
-        <v>2.8309702870502091E-3</v>
+        <v>0.002830970287050209</v>
       </c>
       <c r="K11">
         <v>11.5</v>
@@ -1599,76 +1727,67 @@
       <c r="S11">
         <v>11.5</v>
       </c>
-      <c r="T11" t="str">
-        <f t="shared" si="1"/>
-        <v>777.005316 (11.5)</v>
-      </c>
-      <c r="U11" t="str">
-        <f t="shared" si="2"/>
-        <v>27.874815 (11.5)</v>
-      </c>
-      <c r="V11" t="str">
-        <f t="shared" si="3"/>
-        <v>23.311949 (9.5)</v>
-      </c>
-      <c r="W11" t="str">
-        <f t="shared" si="4"/>
-        <v>0.043266 (9.5)</v>
-      </c>
-      <c r="X11" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.590219 (11.5)</v>
-      </c>
-      <c r="Y11" t="str">
-        <f t="shared" si="6"/>
-        <v>56.56752 (3.5)</v>
-      </c>
-      <c r="Z11" t="str">
-        <f t="shared" si="7"/>
-        <v>0.052584 (11.5)</v>
-      </c>
-      <c r="AA11" t="str">
-        <f t="shared" si="8"/>
-        <v>1.482716 (11.5)</v>
-      </c>
-      <c r="AB11" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002831 (11.5)</v>
-      </c>
-      <c r="AC11" s="2">
+      <c r="T11">
         <v>10.16666666666667</v>
       </c>
+      <c r="U11" t="s">
+        <v>48</v>
+      </c>
+      <c r="V11" t="s">
+        <v>58</v>
+      </c>
+      <c r="W11" t="s">
+        <v>68</v>
+      </c>
+      <c r="X11" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
         <v>39</v>
       </c>
       <c r="B12">
-        <v>717.34680356602132</v>
+        <v>717.3468035660213</v>
       </c>
       <c r="C12">
-        <v>26.783330703368861</v>
+        <v>26.78333070336886</v>
       </c>
       <c r="D12">
-        <v>21.853453570839552</v>
+        <v>21.85345357083955</v>
       </c>
       <c r="E12">
-        <v>4.067794409124053E-2</v>
+        <v>0.04067794409124053</v>
       </c>
       <c r="F12">
-        <v>-0.46812201792964131</v>
+        <v>-0.4681220179296413</v>
       </c>
       <c r="G12">
-        <v>59.761543833688279</v>
+        <v>59.76154383368828</v>
       </c>
       <c r="H12">
-        <v>5.0558654987649589E-2</v>
+        <v>0.05055865498764959</v>
       </c>
       <c r="I12">
         <v>1.368929315589511</v>
       </c>
       <c r="J12">
-        <v>2.6139591512357009E-3</v>
+        <v>0.002613959151235701</v>
       </c>
       <c r="K12">
         <v>8</v>
@@ -1697,76 +1816,67 @@
       <c r="S12">
         <v>8</v>
       </c>
-      <c r="T12" t="str">
-        <f t="shared" si="1"/>
-        <v>717.346804 (8)</v>
-      </c>
-      <c r="U12" t="str">
-        <f t="shared" si="2"/>
-        <v>26.783331 (8)</v>
-      </c>
-      <c r="V12" t="str">
-        <f t="shared" si="3"/>
-        <v>21.853454 (7)</v>
-      </c>
-      <c r="W12" t="str">
-        <f t="shared" si="4"/>
-        <v>0.040678 (7)</v>
-      </c>
-      <c r="X12" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.468122 (8)</v>
-      </c>
-      <c r="Y12" t="str">
-        <f t="shared" si="6"/>
-        <v>59.761544 (6)</v>
-      </c>
-      <c r="Z12" t="str">
-        <f t="shared" si="7"/>
-        <v>0.050559 (8)</v>
-      </c>
-      <c r="AA12" t="str">
-        <f t="shared" si="8"/>
-        <v>1.368929 (8)</v>
-      </c>
-      <c r="AB12" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002614 (8)</v>
-      </c>
-      <c r="AC12" s="2">
-        <v>7.5555555555555554</v>
+      <c r="T12">
+        <v>7.555555555555555</v>
+      </c>
+      <c r="U12" t="s">
+        <v>49</v>
+      </c>
+      <c r="V12" t="s">
+        <v>59</v>
+      </c>
+      <c r="W12" t="s">
+        <v>69</v>
+      </c>
+      <c r="X12" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>40</v>
       </c>
       <c r="B13">
-        <v>810.64730670525512</v>
+        <v>810.6473067052551</v>
       </c>
       <c r="C13">
         <v>28.47186869008171</v>
       </c>
       <c r="D13">
-        <v>23.505499952799688</v>
+        <v>23.50549995279969</v>
       </c>
       <c r="E13">
-        <v>4.3670966376120078E-2</v>
+        <v>0.04367096637612008</v>
       </c>
       <c r="F13">
-        <v>-0.65907083412523182</v>
+        <v>-0.6590708341252318</v>
       </c>
       <c r="G13">
-        <v>60.125137324584841</v>
+        <v>60.12513732458484</v>
       </c>
       <c r="H13">
-        <v>5.3790964099790547E-2</v>
+        <v>0.05379096409979055</v>
       </c>
       <c r="I13">
         <v>1.549436315383161</v>
       </c>
       <c r="J13">
-        <v>2.9632361884829829E-3</v>
+        <v>0.002963236188482983</v>
       </c>
       <c r="K13">
         <v>13</v>
@@ -1795,76 +1905,67 @@
       <c r="S13">
         <v>13</v>
       </c>
-      <c r="T13" t="str">
-        <f t="shared" si="1"/>
-        <v>810.647307 (13)</v>
-      </c>
-      <c r="U13" t="str">
-        <f t="shared" si="2"/>
-        <v>28.471869 (13)</v>
-      </c>
-      <c r="V13" t="str">
-        <f t="shared" si="3"/>
-        <v>23.5055 (13)</v>
-      </c>
-      <c r="W13" t="str">
-        <f t="shared" si="4"/>
-        <v>0.043671 (13)</v>
-      </c>
-      <c r="X13" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.659071 (13)</v>
-      </c>
-      <c r="Y13" t="str">
-        <f t="shared" si="6"/>
-        <v>60.125137 (7)</v>
-      </c>
-      <c r="Z13" t="str">
-        <f t="shared" si="7"/>
-        <v>0.053791 (13)</v>
-      </c>
-      <c r="AA13" t="str">
-        <f t="shared" si="8"/>
-        <v>1.549436 (13)</v>
-      </c>
-      <c r="AB13" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002963 (13)</v>
-      </c>
-      <c r="AC13" s="2">
+      <c r="T13">
         <v>12.33333333333333</v>
       </c>
+      <c r="U13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V13" t="s">
+        <v>60</v>
+      </c>
+      <c r="W13" t="s">
+        <v>70</v>
+      </c>
+      <c r="X13" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
         <v>41</v>
       </c>
       <c r="B14">
-        <v>929.91091680947125</v>
+        <v>929.9109168094712</v>
       </c>
       <c r="C14">
-        <v>30.494440752528501</v>
+        <v>30.4944407525285</v>
       </c>
       <c r="D14">
         <v>25.8341702526007</v>
       </c>
       <c r="E14">
-        <v>4.7939405371417318E-2</v>
+        <v>0.04793940537141732</v>
       </c>
       <c r="F14">
-        <v>-0.90315574683602096</v>
+        <v>-0.903155746836021</v>
       </c>
       <c r="G14">
-        <v>58.763675824182599</v>
+        <v>58.7636758241826</v>
       </c>
       <c r="H14">
-        <v>5.7750116588687277E-2</v>
+        <v>0.05775011658868728</v>
       </c>
       <c r="I14">
         <v>1.783876433246633</v>
       </c>
       <c r="J14">
-        <v>3.4241258201082041E-3</v>
+        <v>0.003424125820108204</v>
       </c>
       <c r="K14">
         <v>15</v>
@@ -1893,76 +1994,67 @@
       <c r="S14">
         <v>15</v>
       </c>
-      <c r="T14" t="str">
-        <f t="shared" si="1"/>
-        <v>929.910917 (15)</v>
-      </c>
-      <c r="U14" t="str">
-        <f t="shared" si="2"/>
-        <v>30.494441 (15)</v>
-      </c>
-      <c r="V14" t="str">
-        <f t="shared" si="3"/>
-        <v>25.83417 (15)</v>
-      </c>
-      <c r="W14" t="str">
-        <f t="shared" si="4"/>
-        <v>0.047939 (15)</v>
-      </c>
-      <c r="X14" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.903156 (15)</v>
-      </c>
-      <c r="Y14" t="str">
-        <f t="shared" si="6"/>
-        <v>58.763676 (5)</v>
-      </c>
-      <c r="Z14" t="str">
-        <f t="shared" si="7"/>
-        <v>0.05775 (15)</v>
-      </c>
-      <c r="AA14" t="str">
-        <f t="shared" si="8"/>
-        <v>1.783876 (15)</v>
-      </c>
-      <c r="AB14" t="str">
-        <f t="shared" si="9"/>
-        <v>0.003424 (15)</v>
-      </c>
-      <c r="AC14" s="2">
-        <v>13.888888888888889</v>
+      <c r="T14">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="U14" t="s">
+        <v>51</v>
+      </c>
+      <c r="V14" t="s">
+        <v>61</v>
+      </c>
+      <c r="W14" t="s">
+        <v>71</v>
+      </c>
+      <c r="X14" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>42</v>
       </c>
       <c r="B15">
-        <v>818.35017501897892</v>
+        <v>818.3501750189789</v>
       </c>
       <c r="C15">
-        <v>28.606820428334551</v>
+        <v>28.60682042833455</v>
       </c>
       <c r="D15">
-        <v>23.990441641161841</v>
+        <v>23.99044164116184</v>
       </c>
       <c r="E15">
-        <v>4.4533518247760522E-2</v>
+        <v>0.04453351824776052</v>
       </c>
       <c r="F15">
-        <v>-0.67483552495032972</v>
+        <v>-0.6748355249503297</v>
       </c>
       <c r="G15">
-        <v>60.170630607549192</v>
+        <v>60.17063060754919</v>
       </c>
       <c r="H15">
-        <v>5.4027721123280602E-2</v>
+        <v>0.0540277211232806</v>
       </c>
       <c r="I15">
-        <v>1.5639871406672949</v>
+        <v>1.563987140667295</v>
       </c>
       <c r="J15">
-        <v>2.9907134343519098E-3</v>
+        <v>0.00299071343435191</v>
       </c>
       <c r="K15">
         <v>14</v>
@@ -1991,76 +2083,67 @@
       <c r="S15">
         <v>14</v>
       </c>
-      <c r="T15" t="str">
-        <f t="shared" si="1"/>
-        <v>818.350175 (14)</v>
-      </c>
-      <c r="U15" t="str">
-        <f t="shared" si="2"/>
-        <v>28.60682 (14)</v>
-      </c>
-      <c r="V15" t="str">
-        <f t="shared" si="3"/>
-        <v>23.990442 (14)</v>
-      </c>
-      <c r="W15" t="str">
-        <f t="shared" si="4"/>
-        <v>0.044534 (14)</v>
-      </c>
-      <c r="X15" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.674836 (14)</v>
-      </c>
-      <c r="Y15" t="str">
-        <f t="shared" si="6"/>
-        <v>60.170631 (8)</v>
-      </c>
-      <c r="Z15" t="str">
-        <f t="shared" si="7"/>
-        <v>0.054028 (14)</v>
-      </c>
-      <c r="AA15" t="str">
-        <f t="shared" si="8"/>
-        <v>1.563987 (14)</v>
-      </c>
-      <c r="AB15" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002991 (14)</v>
-      </c>
-      <c r="AC15" s="2">
+      <c r="T15">
         <v>13.33333333333333</v>
       </c>
+      <c r="U15" t="s">
+        <v>52</v>
+      </c>
+      <c r="V15" t="s">
+        <v>62</v>
+      </c>
+      <c r="W15" t="s">
+        <v>72</v>
+      </c>
+      <c r="X15" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16">
-        <v>691.13156727857097</v>
+        <v>691.131567278571</v>
       </c>
       <c r="C16">
-        <v>26.289381264658381</v>
+        <v>26.28938126465838</v>
       </c>
       <c r="D16">
-        <v>21.954650461802579</v>
+        <v>21.95465046180258</v>
       </c>
       <c r="E16">
-        <v>4.0889470885861083E-2</v>
+        <v>0.04088947088586108</v>
       </c>
       <c r="F16">
-        <v>-0.41446991352559359</v>
+        <v>-0.4144699135255936</v>
       </c>
       <c r="G16">
-        <v>60.914562351273162</v>
+        <v>60.91456235127316</v>
       </c>
       <c r="H16">
-        <v>4.9628098204403732E-2</v>
+        <v>0.04962809820440373</v>
       </c>
       <c r="I16">
         <v>1.318155836806822</v>
       </c>
       <c r="J16">
-        <v>2.5156385408683E-3</v>
+        <v>0.0025156385408683</v>
       </c>
       <c r="K16">
         <v>7</v>
@@ -2089,53 +2172,38 @@
       <c r="S16">
         <v>7</v>
       </c>
-      <c r="T16" t="str">
-        <f t="shared" si="1"/>
-        <v>691.131567 (7)</v>
-      </c>
-      <c r="U16" t="str">
-        <f t="shared" si="2"/>
-        <v>26.289381 (7)</v>
-      </c>
-      <c r="V16" t="str">
-        <f t="shared" si="3"/>
-        <v>21.95465 (8)</v>
-      </c>
-      <c r="W16" t="str">
-        <f t="shared" si="4"/>
-        <v>0.040889 (8)</v>
-      </c>
-      <c r="X16" t="str">
-        <f t="shared" si="5"/>
-        <v>-0.41447 (7)</v>
-      </c>
-      <c r="Y16" t="str">
-        <f t="shared" si="6"/>
-        <v>60.914562 (9)</v>
-      </c>
-      <c r="Z16" t="str">
-        <f t="shared" si="7"/>
-        <v>0.049628 (7)</v>
-      </c>
-      <c r="AA16" t="str">
-        <f t="shared" si="8"/>
-        <v>1.318156 (7)</v>
-      </c>
-      <c r="AB16" t="str">
-        <f t="shared" si="9"/>
-        <v>0.002516 (7)</v>
-      </c>
-      <c r="AC16" s="2">
-        <v>7.4444444444444446</v>
+      <c r="T16">
+        <v>7.444444444444445</v>
+      </c>
+      <c r="U16" t="s">
+        <v>53</v>
+      </c>
+      <c r="V16" t="s">
+        <v>63</v>
+      </c>
+      <c r="W16" t="s">
+        <v>73</v>
+      </c>
+      <c r="X16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:S16">
-    <cfRule type="top10" dxfId="2" priority="2" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC16">
-    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>